<commit_message>
bug fixes / feature additions / verbosity
</commit_message>
<xml_diff>
--- a/examples/sop/data/metadata.xlsx
+++ b/examples/sop/data/metadata.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Andi/Development/MG-RAST-Repo/MG-RAST-Tools/examples/sop/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="460" windowWidth="32700" windowHeight="18400" activeTab="1"/>
   </bookViews>
@@ -18,13 +13,13 @@
     <sheet name="library metagenome" sheetId="4" r:id="rId4"/>
     <sheet name="ep soil" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -870,9 +865,6 @@
     <t>5. Library field 'metagenome_name' must be unique for each library, and will be the name of the MG-RAST metagenome</t>
   </si>
   <si>
-    <t>Demo Project</t>
-  </si>
-  <si>
     <t>Metagenomic data from  a demo site</t>
   </si>
   <si>
@@ -907,6 +899,9 @@
   </si>
   <si>
     <t>principle.investigator@lab.no.where</t>
+  </si>
+  <si>
+    <t>Demo Project 2</t>
   </si>
 </sst>
 </file>
@@ -916,7 +911,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -928,6 +923,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -950,9 +953,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -960,7 +964,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1017,7 +1022,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -1052,7 +1057,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -1265,80 +1270,85 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1">
       <c r="A4" s="1" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1">
       <c r="A8" s="1" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1">
       <c r="A9" s="1" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1">
       <c r="A10" s="1" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1">
       <c r="A12" s="1" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1">
       <c r="A13" s="1" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1">
       <c r="A14" s="1" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1">
       <c r="A15" s="1" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1">
       <c r="A16" s="1" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
         <v>278</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1347,12 +1357,12 @@
   <dimension ref="A1:Y3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
         <v>215</v>
       </c>
@@ -1429,7 +1439,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25">
       <c r="A2" s="1" t="s">
         <v>239</v>
       </c>
@@ -1506,36 +1516,36 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25">
       <c r="A3" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>280</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>263</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>282</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>200</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>264</v>
@@ -1546,6 +1556,11 @@
     <hyperlink ref="E3" r:id="rId1" display="principle.investigator@lab.org"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1553,13 +1568,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB144"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1645,7 +1660,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28">
       <c r="A2" s="1" t="s">
         <v>174</v>
       </c>
@@ -1731,10 +1746,11 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28">
       <c r="A3" s="1" t="s">
-        <v>284</v>
-      </c>
+        <v>283</v>
+      </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="1">
         <v>44.041719999999998</v>
       </c>
@@ -1772,10 +1788,11 @@
         <v>205</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28">
       <c r="A4" s="1" t="s">
-        <v>285</v>
-      </c>
+        <v>284</v>
+      </c>
+      <c r="B4" s="1"/>
       <c r="C4" s="1">
         <v>40.85089</v>
       </c>
@@ -1813,7 +1830,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28">
       <c r="A5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -1828,7 +1845,7 @@
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28">
       <c r="A6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -1843,7 +1860,7 @@
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28">
       <c r="A7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1858,7 +1875,7 @@
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28">
       <c r="A8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1873,7 +1890,7 @@
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28">
       <c r="A9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1888,7 +1905,7 @@
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28">
       <c r="A10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1903,7 +1920,7 @@
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28">
       <c r="A11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1918,7 +1935,7 @@
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28">
       <c r="A12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1933,7 +1950,7 @@
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28">
       <c r="A13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1948,7 +1965,7 @@
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28">
       <c r="A14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1963,7 +1980,7 @@
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28">
       <c r="A15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1978,7 +1995,7 @@
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28">
       <c r="A16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1993,7 +2010,7 @@
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27">
       <c r="A17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -2008,7 +2025,7 @@
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27">
       <c r="A18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -2023,7 +2040,7 @@
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27">
       <c r="A19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -2038,7 +2055,7 @@
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27">
       <c r="A20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2053,7 +2070,7 @@
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27">
       <c r="A21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -2068,7 +2085,7 @@
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27">
       <c r="A22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -2083,7 +2100,7 @@
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27">
       <c r="A23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -2098,7 +2115,7 @@
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27">
       <c r="A24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -2113,7 +2130,7 @@
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27">
       <c r="A25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -2128,7 +2145,7 @@
       <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27">
       <c r="A26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -2143,7 +2160,7 @@
       <c r="Z26" s="1"/>
       <c r="AA26" s="1"/>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27">
       <c r="A27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -2158,7 +2175,7 @@
       <c r="Z27" s="1"/>
       <c r="AA27" s="1"/>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27">
       <c r="A28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -2173,7 +2190,7 @@
       <c r="Z28" s="1"/>
       <c r="AA28" s="1"/>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27">
       <c r="A29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -2188,7 +2205,7 @@
       <c r="Z29" s="1"/>
       <c r="AA29" s="1"/>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27">
       <c r="A30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -2203,7 +2220,7 @@
       <c r="Z30" s="1"/>
       <c r="AA30" s="1"/>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27">
       <c r="A31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -2218,7 +2235,7 @@
       <c r="Z31" s="1"/>
       <c r="AA31" s="1"/>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27">
       <c r="A32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -2233,7 +2250,7 @@
       <c r="Z32" s="1"/>
       <c r="AA32" s="1"/>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:27">
       <c r="A33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -2248,7 +2265,7 @@
       <c r="Z33" s="1"/>
       <c r="AA33" s="1"/>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:27">
       <c r="A34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -2263,7 +2280,7 @@
       <c r="Z34" s="1"/>
       <c r="AA34" s="1"/>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:27">
       <c r="A35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -2278,7 +2295,7 @@
       <c r="Z35" s="1"/>
       <c r="AA35" s="1"/>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:27">
       <c r="A36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -2293,7 +2310,7 @@
       <c r="Z36" s="1"/>
       <c r="AA36" s="1"/>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:27">
       <c r="A37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -2308,7 +2325,7 @@
       <c r="Z37" s="1"/>
       <c r="AA37" s="1"/>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:27">
       <c r="A38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -2323,7 +2340,7 @@
       <c r="Z38" s="1"/>
       <c r="AA38" s="1"/>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:27">
       <c r="A39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -2338,7 +2355,7 @@
       <c r="Z39" s="1"/>
       <c r="AA39" s="1"/>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:27">
       <c r="A40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -2353,7 +2370,7 @@
       <c r="Z40" s="1"/>
       <c r="AA40" s="1"/>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:27">
       <c r="A41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -2368,7 +2385,7 @@
       <c r="Z41" s="1"/>
       <c r="AA41" s="1"/>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:27">
       <c r="A42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -2383,7 +2400,7 @@
       <c r="Z42" s="1"/>
       <c r="AA42" s="1"/>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:27">
       <c r="A43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -2398,7 +2415,7 @@
       <c r="Z43" s="1"/>
       <c r="AA43" s="1"/>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:27">
       <c r="A44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -2413,7 +2430,7 @@
       <c r="Z44" s="1"/>
       <c r="AA44" s="1"/>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:27">
       <c r="A45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -2428,7 +2445,7 @@
       <c r="Z45" s="1"/>
       <c r="AA45" s="1"/>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:27">
       <c r="A46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -2443,7 +2460,7 @@
       <c r="Z46" s="1"/>
       <c r="AA46" s="1"/>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:27">
       <c r="A47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -2458,7 +2475,7 @@
       <c r="Z47" s="1"/>
       <c r="AA47" s="1"/>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:27">
       <c r="A48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -2473,7 +2490,7 @@
       <c r="Z48" s="1"/>
       <c r="AA48" s="1"/>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:27">
       <c r="A49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -2488,7 +2505,7 @@
       <c r="Z49" s="1"/>
       <c r="AA49" s="1"/>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:27">
       <c r="A50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -2503,7 +2520,7 @@
       <c r="Z50" s="1"/>
       <c r="AA50" s="1"/>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:27">
       <c r="A51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -2518,7 +2535,7 @@
       <c r="Z51" s="1"/>
       <c r="AA51" s="1"/>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:27">
       <c r="A52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -2533,7 +2550,7 @@
       <c r="Z52" s="1"/>
       <c r="AA52" s="1"/>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:27">
       <c r="A53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -2548,7 +2565,7 @@
       <c r="Z53" s="1"/>
       <c r="AA53" s="1"/>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:27">
       <c r="A54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -2563,7 +2580,7 @@
       <c r="Z54" s="1"/>
       <c r="AA54" s="1"/>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:27">
       <c r="A55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -2578,7 +2595,7 @@
       <c r="Z55" s="1"/>
       <c r="AA55" s="1"/>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:27">
       <c r="A56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -2593,7 +2610,7 @@
       <c r="Z56" s="1"/>
       <c r="AA56" s="1"/>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:27">
       <c r="A57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -2608,7 +2625,7 @@
       <c r="Z57" s="1"/>
       <c r="AA57" s="1"/>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:27">
       <c r="A58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -2623,7 +2640,7 @@
       <c r="Z58" s="1"/>
       <c r="AA58" s="1"/>
     </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:27">
       <c r="A59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -2638,7 +2655,7 @@
       <c r="Z59" s="1"/>
       <c r="AA59" s="1"/>
     </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:27">
       <c r="A60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -2653,7 +2670,7 @@
       <c r="Z60" s="1"/>
       <c r="AA60" s="1"/>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:27">
       <c r="A61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -2668,7 +2685,7 @@
       <c r="Z61" s="1"/>
       <c r="AA61" s="1"/>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:27">
       <c r="A62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -2683,7 +2700,7 @@
       <c r="Z62" s="1"/>
       <c r="AA62" s="1"/>
     </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:27">
       <c r="A63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -2698,7 +2715,7 @@
       <c r="Z63" s="1"/>
       <c r="AA63" s="1"/>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:27">
       <c r="A64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -2713,7 +2730,7 @@
       <c r="Z64" s="1"/>
       <c r="AA64" s="1"/>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:27">
       <c r="A65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -2728,7 +2745,7 @@
       <c r="Z65" s="1"/>
       <c r="AA65" s="1"/>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:27">
       <c r="A66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -2743,7 +2760,7 @@
       <c r="Z66" s="1"/>
       <c r="AA66" s="1"/>
     </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:27">
       <c r="A67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -2758,7 +2775,7 @@
       <c r="Z67" s="1"/>
       <c r="AA67" s="1"/>
     </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:27">
       <c r="A68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -2773,7 +2790,7 @@
       <c r="Z68" s="1"/>
       <c r="AA68" s="1"/>
     </row>
-    <row r="69" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:27">
       <c r="A69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -2788,7 +2805,7 @@
       <c r="Z69" s="1"/>
       <c r="AA69" s="1"/>
     </row>
-    <row r="70" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:27">
       <c r="A70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -2803,7 +2820,7 @@
       <c r="Z70" s="1"/>
       <c r="AA70" s="1"/>
     </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:27">
       <c r="A71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -2818,7 +2835,7 @@
       <c r="Z71" s="1"/>
       <c r="AA71" s="1"/>
     </row>
-    <row r="72" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:27">
       <c r="A72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -2833,7 +2850,7 @@
       <c r="Z72" s="1"/>
       <c r="AA72" s="1"/>
     </row>
-    <row r="73" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:27">
       <c r="A73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
@@ -2848,7 +2865,7 @@
       <c r="Z73" s="1"/>
       <c r="AA73" s="1"/>
     </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:27">
       <c r="A74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -2863,7 +2880,7 @@
       <c r="Z74" s="1"/>
       <c r="AA74" s="1"/>
     </row>
-    <row r="75" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:27">
       <c r="A75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -2878,7 +2895,7 @@
       <c r="Z75" s="1"/>
       <c r="AA75" s="1"/>
     </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:27">
       <c r="A76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -2893,7 +2910,7 @@
       <c r="Z76" s="1"/>
       <c r="AA76" s="1"/>
     </row>
-    <row r="77" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:27">
       <c r="A77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -2908,7 +2925,7 @@
       <c r="Z77" s="1"/>
       <c r="AA77" s="1"/>
     </row>
-    <row r="78" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:27">
       <c r="A78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -2923,7 +2940,7 @@
       <c r="Z78" s="1"/>
       <c r="AA78" s="1"/>
     </row>
-    <row r="79" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:27">
       <c r="A79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
@@ -2938,7 +2955,7 @@
       <c r="Z79" s="1"/>
       <c r="AA79" s="1"/>
     </row>
-    <row r="80" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:27">
       <c r="A80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
@@ -2953,7 +2970,7 @@
       <c r="Z80" s="1"/>
       <c r="AA80" s="1"/>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:27">
       <c r="A81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
@@ -2968,7 +2985,7 @@
       <c r="Z81" s="1"/>
       <c r="AA81" s="1"/>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:27">
       <c r="A82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
@@ -2983,7 +3000,7 @@
       <c r="Z82" s="1"/>
       <c r="AA82" s="1"/>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:27">
       <c r="A83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
@@ -2998,7 +3015,7 @@
       <c r="Z83" s="1"/>
       <c r="AA83" s="1"/>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:27">
       <c r="A84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
@@ -3013,7 +3030,7 @@
       <c r="Z84" s="1"/>
       <c r="AA84" s="1"/>
     </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:27">
       <c r="A85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
@@ -3028,7 +3045,7 @@
       <c r="Z85" s="1"/>
       <c r="AA85" s="1"/>
     </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:27">
       <c r="A86" s="1"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
@@ -3043,7 +3060,7 @@
       <c r="Z86" s="1"/>
       <c r="AA86" s="1"/>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:27">
       <c r="A87" s="1"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
@@ -3058,7 +3075,7 @@
       <c r="Z87" s="1"/>
       <c r="AA87" s="1"/>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:27">
       <c r="A88" s="1"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
@@ -3073,7 +3090,7 @@
       <c r="Z88" s="1"/>
       <c r="AA88" s="1"/>
     </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:27">
       <c r="A89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
@@ -3088,7 +3105,7 @@
       <c r="Z89" s="1"/>
       <c r="AA89" s="1"/>
     </row>
-    <row r="90" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:27">
       <c r="A90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
@@ -3103,7 +3120,7 @@
       <c r="Z90" s="1"/>
       <c r="AA90" s="1"/>
     </row>
-    <row r="91" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:27">
       <c r="A91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
@@ -3118,7 +3135,7 @@
       <c r="Z91" s="1"/>
       <c r="AA91" s="1"/>
     </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:27">
       <c r="A92" s="1"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
@@ -3133,7 +3150,7 @@
       <c r="Z92" s="1"/>
       <c r="AA92" s="1"/>
     </row>
-    <row r="93" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:27">
       <c r="A93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
@@ -3148,7 +3165,7 @@
       <c r="Z93" s="1"/>
       <c r="AA93" s="1"/>
     </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:27">
       <c r="A94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
@@ -3163,7 +3180,7 @@
       <c r="Z94" s="1"/>
       <c r="AA94" s="1"/>
     </row>
-    <row r="95" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:27">
       <c r="A95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
@@ -3178,7 +3195,7 @@
       <c r="Z95" s="1"/>
       <c r="AA95" s="1"/>
     </row>
-    <row r="96" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:27">
       <c r="A96" s="1"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
@@ -3193,7 +3210,7 @@
       <c r="Z96" s="1"/>
       <c r="AA96" s="1"/>
     </row>
-    <row r="97" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:27">
       <c r="A97" s="1"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
@@ -3208,7 +3225,7 @@
       <c r="Z97" s="1"/>
       <c r="AA97" s="1"/>
     </row>
-    <row r="98" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:27">
       <c r="A98" s="1"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
@@ -3223,7 +3240,7 @@
       <c r="Z98" s="1"/>
       <c r="AA98" s="1"/>
     </row>
-    <row r="99" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:27">
       <c r="A99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
@@ -3238,7 +3255,7 @@
       <c r="Z99" s="1"/>
       <c r="AA99" s="1"/>
     </row>
-    <row r="100" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:27">
       <c r="A100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
@@ -3253,7 +3270,7 @@
       <c r="Z100" s="1"/>
       <c r="AA100" s="1"/>
     </row>
-    <row r="101" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:27">
       <c r="A101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
@@ -3268,7 +3285,7 @@
       <c r="Z101" s="1"/>
       <c r="AA101" s="1"/>
     </row>
-    <row r="102" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:27">
       <c r="A102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
@@ -3283,7 +3300,7 @@
       <c r="Z102" s="1"/>
       <c r="AA102" s="1"/>
     </row>
-    <row r="103" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:27">
       <c r="A103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
@@ -3298,7 +3315,7 @@
       <c r="Z103" s="1"/>
       <c r="AA103" s="1"/>
     </row>
-    <row r="104" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:27">
       <c r="A104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
@@ -3313,7 +3330,7 @@
       <c r="Z104" s="1"/>
       <c r="AA104" s="1"/>
     </row>
-    <row r="105" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:27">
       <c r="A105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
@@ -3328,7 +3345,7 @@
       <c r="Z105" s="1"/>
       <c r="AA105" s="1"/>
     </row>
-    <row r="106" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:27">
       <c r="A106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
@@ -3343,7 +3360,7 @@
       <c r="Z106" s="1"/>
       <c r="AA106" s="1"/>
     </row>
-    <row r="107" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:27">
       <c r="A107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
@@ -3358,7 +3375,7 @@
       <c r="Z107" s="1"/>
       <c r="AA107" s="1"/>
     </row>
-    <row r="108" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:27">
       <c r="A108" s="1"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
@@ -3373,7 +3390,7 @@
       <c r="Z108" s="1"/>
       <c r="AA108" s="1"/>
     </row>
-    <row r="109" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:27">
       <c r="A109" s="1"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
@@ -3388,7 +3405,7 @@
       <c r="Z109" s="1"/>
       <c r="AA109" s="1"/>
     </row>
-    <row r="110" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:27">
       <c r="A110" s="1"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
@@ -3403,7 +3420,7 @@
       <c r="Z110" s="1"/>
       <c r="AA110" s="1"/>
     </row>
-    <row r="111" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:27">
       <c r="A111" s="1"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
@@ -3418,7 +3435,7 @@
       <c r="Z111" s="1"/>
       <c r="AA111" s="1"/>
     </row>
-    <row r="112" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:27">
       <c r="A112" s="1"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
@@ -3433,7 +3450,7 @@
       <c r="Z112" s="1"/>
       <c r="AA112" s="1"/>
     </row>
-    <row r="113" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:27">
       <c r="A113" s="1"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
@@ -3448,7 +3465,7 @@
       <c r="Z113" s="1"/>
       <c r="AA113" s="1"/>
     </row>
-    <row r="114" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:27">
       <c r="A114" s="1"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
@@ -3463,7 +3480,7 @@
       <c r="Z114" s="1"/>
       <c r="AA114" s="1"/>
     </row>
-    <row r="115" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:27">
       <c r="A115" s="1"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
@@ -3478,7 +3495,7 @@
       <c r="Z115" s="1"/>
       <c r="AA115" s="1"/>
     </row>
-    <row r="116" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:27">
       <c r="A116" s="1"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
@@ -3493,7 +3510,7 @@
       <c r="Z116" s="1"/>
       <c r="AA116" s="1"/>
     </row>
-    <row r="117" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:27">
       <c r="A117" s="1"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
@@ -3508,7 +3525,7 @@
       <c r="Z117" s="1"/>
       <c r="AA117" s="1"/>
     </row>
-    <row r="118" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:27">
       <c r="A118" s="1"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
@@ -3523,7 +3540,7 @@
       <c r="Z118" s="1"/>
       <c r="AA118" s="1"/>
     </row>
-    <row r="119" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:27">
       <c r="A119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
@@ -3538,7 +3555,7 @@
       <c r="Z119" s="1"/>
       <c r="AA119" s="1"/>
     </row>
-    <row r="120" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:27">
       <c r="A120" s="1"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
@@ -3553,7 +3570,7 @@
       <c r="Z120" s="1"/>
       <c r="AA120" s="1"/>
     </row>
-    <row r="121" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:27">
       <c r="A121" s="1"/>
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
@@ -3568,7 +3585,7 @@
       <c r="Z121" s="1"/>
       <c r="AA121" s="1"/>
     </row>
-    <row r="122" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:27">
       <c r="A122" s="1"/>
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
@@ -3583,7 +3600,7 @@
       <c r="Z122" s="1"/>
       <c r="AA122" s="1"/>
     </row>
-    <row r="123" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:27">
       <c r="A123" s="1"/>
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
@@ -3598,7 +3615,7 @@
       <c r="Z123" s="1"/>
       <c r="AA123" s="1"/>
     </row>
-    <row r="124" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:27">
       <c r="A124" s="1"/>
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
@@ -3613,7 +3630,7 @@
       <c r="Z124" s="1"/>
       <c r="AA124" s="1"/>
     </row>
-    <row r="125" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:27">
       <c r="A125" s="1"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
@@ -3628,7 +3645,7 @@
       <c r="Z125" s="1"/>
       <c r="AA125" s="1"/>
     </row>
-    <row r="126" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:27">
       <c r="A126" s="1"/>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
@@ -3643,7 +3660,7 @@
       <c r="Z126" s="1"/>
       <c r="AA126" s="1"/>
     </row>
-    <row r="127" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:27">
       <c r="A127" s="1"/>
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
@@ -3658,7 +3675,7 @@
       <c r="Z127" s="1"/>
       <c r="AA127" s="1"/>
     </row>
-    <row r="128" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:27">
       <c r="A128" s="1"/>
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
@@ -3673,7 +3690,7 @@
       <c r="Z128" s="1"/>
       <c r="AA128" s="1"/>
     </row>
-    <row r="129" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:27">
       <c r="A129" s="1"/>
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
@@ -3688,7 +3705,7 @@
       <c r="Z129" s="1"/>
       <c r="AA129" s="1"/>
     </row>
-    <row r="130" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:27">
       <c r="A130" s="1"/>
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
@@ -3703,7 +3720,7 @@
       <c r="Z130" s="1"/>
       <c r="AA130" s="1"/>
     </row>
-    <row r="131" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:27">
       <c r="A131" s="1"/>
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
@@ -3718,7 +3735,7 @@
       <c r="Z131" s="1"/>
       <c r="AA131" s="1"/>
     </row>
-    <row r="132" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:27">
       <c r="A132" s="1"/>
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
@@ -3733,7 +3750,7 @@
       <c r="Z132" s="1"/>
       <c r="AA132" s="1"/>
     </row>
-    <row r="133" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:27">
       <c r="A133" s="1"/>
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
@@ -3748,7 +3765,7 @@
       <c r="Z133" s="1"/>
       <c r="AA133" s="1"/>
     </row>
-    <row r="134" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:27">
       <c r="A134" s="1"/>
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
@@ -3763,7 +3780,7 @@
       <c r="Z134" s="1"/>
       <c r="AA134" s="1"/>
     </row>
-    <row r="135" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:27">
       <c r="A135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
@@ -3778,7 +3795,7 @@
       <c r="Z135" s="1"/>
       <c r="AA135" s="1"/>
     </row>
-    <row r="136" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:27">
       <c r="A136" s="1"/>
       <c r="C136" s="1"/>
       <c r="D136" s="1"/>
@@ -3793,7 +3810,7 @@
       <c r="Z136" s="1"/>
       <c r="AA136" s="1"/>
     </row>
-    <row r="137" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:27">
       <c r="A137" s="1"/>
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
@@ -3808,7 +3825,7 @@
       <c r="Z137" s="1"/>
       <c r="AA137" s="1"/>
     </row>
-    <row r="138" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:27">
       <c r="A138" s="1"/>
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
@@ -3823,7 +3840,7 @@
       <c r="Z138" s="1"/>
       <c r="AA138" s="1"/>
     </row>
-    <row r="139" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:27">
       <c r="A139" s="1"/>
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
@@ -3838,7 +3855,7 @@
       <c r="Z139" s="1"/>
       <c r="AA139" s="1"/>
     </row>
-    <row r="140" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:27">
       <c r="A140" s="1"/>
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
@@ -3853,7 +3870,7 @@
       <c r="Z140" s="1"/>
       <c r="AA140" s="1"/>
     </row>
-    <row r="141" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:27">
       <c r="A141" s="1"/>
       <c r="C141" s="1"/>
       <c r="D141" s="1"/>
@@ -3868,7 +3885,7 @@
       <c r="Z141" s="1"/>
       <c r="AA141" s="1"/>
     </row>
-    <row r="142" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:27">
       <c r="A142" s="1"/>
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
@@ -3883,7 +3900,7 @@
       <c r="Z142" s="1"/>
       <c r="AA142" s="1"/>
     </row>
-    <row r="143" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:27">
       <c r="A143" s="1"/>
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
@@ -3898,7 +3915,7 @@
       <c r="Z143" s="1"/>
       <c r="AA143" s="1"/>
     </row>
-    <row r="144" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:27">
       <c r="A144" s="1"/>
       <c r="C144" s="1"/>
       <c r="D144" s="1"/>
@@ -3915,6 +3932,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3923,12 +3945,12 @@
   <dimension ref="A1:Z144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4008,7 +4030,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26">
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
@@ -4088,12 +4110,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26">
       <c r="A3" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>147</v>
@@ -4102,15 +4124,15 @@
         <v>148</v>
       </c>
       <c r="E3" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
       <c r="A4" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>285</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>286</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>147</v>
@@ -4119,844 +4141,844 @@
         <v>148</v>
       </c>
       <c r="E4" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
       <c r="D136" s="1"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
       <c r="D141" s="1"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -4964,6 +4986,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4975,9 +5003,9 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:50">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5129,7 +5157,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:50">
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
@@ -5281,437 +5309,442 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:50">
       <c r="A3" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="4" spans="1:50">
+      <c r="A4" s="1" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:50">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:50">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:50">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:50">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:50">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:50">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:50">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:50">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:50">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:50">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:50">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:50">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1">
       <c r="A39" s="1"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1">
       <c r="A48" s="1"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1">
       <c r="A49" s="1"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1">
       <c r="A50" s="1"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1">
       <c r="A51" s="1"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1">
       <c r="A53" s="1"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1">
       <c r="A54" s="1"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1">
       <c r="A55" s="1"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1">
       <c r="A58" s="1"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1">
       <c r="A59" s="1"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1">
       <c r="A60" s="1"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1">
       <c r="A61" s="1"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1">
       <c r="A62" s="1"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1">
       <c r="A63" s="1"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1">
       <c r="A64" s="1"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1">
       <c r="A65" s="1"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1">
       <c r="A66" s="1"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1">
       <c r="A67" s="1"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1">
       <c r="A68" s="1"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1">
       <c r="A69" s="1"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1">
       <c r="A70" s="1"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1">
       <c r="A71" s="1"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1">
       <c r="A72" s="1"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1">
       <c r="A73" s="1"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1">
       <c r="A74" s="1"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1">
       <c r="A75" s="1"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1">
       <c r="A76" s="1"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1">
       <c r="A77" s="1"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1">
       <c r="A78" s="1"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1">
       <c r="A79" s="1"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1">
       <c r="A80" s="1"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1">
       <c r="A81" s="1"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1">
       <c r="A82" s="1"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1">
       <c r="A83" s="1"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1">
       <c r="A84" s="1"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1">
       <c r="A85" s="1"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1">
       <c r="A86" s="1"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1">
       <c r="A87" s="1"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1">
       <c r="A88" s="1"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1">
       <c r="A89" s="1"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1">
       <c r="A90" s="1"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1">
       <c r="A91" s="1"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1">
       <c r="A92" s="1"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1">
       <c r="A93" s="1"/>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1">
       <c r="A94" s="1"/>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1">
       <c r="A95" s="1"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1">
       <c r="A96" s="1"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1">
       <c r="A97" s="1"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1">
       <c r="A98" s="1"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1">
       <c r="A99" s="1"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1">
       <c r="A100" s="1"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1">
       <c r="A101" s="1"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1">
       <c r="A102" s="1"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1">
       <c r="A103" s="1"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1">
       <c r="A104" s="1"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1">
       <c r="A105" s="1"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1">
       <c r="A106" s="1"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1">
       <c r="A107" s="1"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1">
       <c r="A108" s="1"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1">
       <c r="A109" s="1"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1">
       <c r="A110" s="1"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1">
       <c r="A111" s="1"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1">
       <c r="A112" s="1"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1">
       <c r="A113" s="1"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1">
       <c r="A114" s="1"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1">
       <c r="A115" s="1"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1">
       <c r="A116" s="1"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1">
       <c r="A117" s="1"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1">
       <c r="A118" s="1"/>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1">
       <c r="A119" s="1"/>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1">
       <c r="A120" s="1"/>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1">
       <c r="A121" s="1"/>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1">
       <c r="A122" s="1"/>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1">
       <c r="A123" s="1"/>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1">
       <c r="A124" s="1"/>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1">
       <c r="A125" s="1"/>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1">
       <c r="A126" s="1"/>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1">
       <c r="A127" s="1"/>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1">
       <c r="A128" s="1"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1">
       <c r="A129" s="1"/>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1">
       <c r="A130" s="1"/>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1">
       <c r="A131" s="1"/>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1">
       <c r="A132" s="1"/>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:1">
       <c r="A133" s="1"/>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:1">
       <c r="A134" s="1"/>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:1">
       <c r="A135" s="1"/>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:1">
       <c r="A136" s="1"/>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:1">
       <c r="A137" s="1"/>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:1">
       <c r="A138" s="1"/>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:1">
       <c r="A139" s="1"/>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:1">
       <c r="A140" s="1"/>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:1">
       <c r="A141" s="1"/>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:1">
       <c r="A142" s="1"/>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:1">
       <c r="A143" s="1"/>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:1">
       <c r="A144" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>